<commit_message>
fig captions and SHC excel files
Changed captions of SigClust figures to first show the method name (hard, soft, sample, true)

Also new SHC excel files; similar to tables in thesis - make more sense than previous tables
</commit_message>
<xml_diff>
--- a/SHC code/sims/K_2_signal_1st_dir.xlsx
+++ b/SHC code/sims/K_2_signal_1st_dir.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Steve\Documents\GitHub\thesis\SHC code\sims\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{301B71D5-19D2-457A-8648-46B572E4B257}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B1CCF6C-9A5A-461D-9C2B-AF3F09481491}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{9CA45C61-1169-4AC7-9660-1FA924585924}"/>
   </bookViews>
@@ -66,9 +66,6 @@
     <t>True $K$</t>
   </si>
   <si>
-    <t>Median time (sec.)</t>
-  </si>
-  <si>
     <t>Simulation Settings</t>
   </si>
   <si>
@@ -289,6 +286,9 @@
   </si>
   <si>
     <t>1st dir.</t>
+  </si>
+  <si>
+    <t>Median time for 1 replication (sec.)</t>
   </si>
 </sst>
 </file>
@@ -414,15 +414,6 @@
   </cellStyleXfs>
   <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -440,6 +431,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -757,68 +757,68 @@
   <dimension ref="A1:L77"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="2"/>
-      <c r="F1" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="G1" s="1"/>
-      <c r="H1" s="3" t="s">
+      <c r="A1" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" s="10"/>
+      <c r="C1" s="10"/>
+      <c r="D1" s="10"/>
+      <c r="E1" s="11"/>
+      <c r="F1" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="G1" s="10"/>
+      <c r="H1" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="I1" s="1"/>
-      <c r="J1" s="1"/>
-      <c r="K1" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="L1" s="1"/>
+      <c r="I1" s="10"/>
+      <c r="J1" s="10"/>
+      <c r="K1" s="12" t="s">
+        <v>84</v>
+      </c>
+      <c r="L1" s="10"/>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="D2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="E2" s="4" t="s">
+      <c r="E2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="F2" s="5" t="s">
+      <c r="F2" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="G2" s="6" t="s">
+      <c r="G2" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="H2" s="4" t="s">
+      <c r="H2" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="I2" s="4" t="s">
+      <c r="I2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="J2" s="7" t="s">
+      <c r="J2" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="K2" s="9" t="s">
+      <c r="K2" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="L2" s="8" t="s">
+      <c r="L2" s="5" t="s">
         <v>8</v>
       </c>
     </row>
@@ -833,16 +833,16 @@
         <v>2</v>
       </c>
       <c r="D3" t="s">
-        <v>83</v>
-      </c>
-      <c r="E3" s="10" t="s">
-        <v>84</v>
+        <v>82</v>
+      </c>
+      <c r="E3" s="7" t="s">
+        <v>83</v>
       </c>
       <c r="F3" t="s">
-        <v>12</v>
-      </c>
-      <c r="G3" s="10" t="s">
-        <v>12</v>
+        <v>11</v>
+      </c>
+      <c r="G3" s="7" t="s">
+        <v>11</v>
       </c>
       <c r="H3">
         <v>0</v>
@@ -850,7 +850,7 @@
       <c r="I3">
         <v>0</v>
       </c>
-      <c r="J3" s="10">
+      <c r="J3" s="7">
         <v>0</v>
       </c>
       <c r="K3">
@@ -871,16 +871,16 @@
         <v>4</v>
       </c>
       <c r="D4" t="s">
-        <v>83</v>
-      </c>
-      <c r="E4" s="11" t="s">
-        <v>84</v>
+        <v>82</v>
+      </c>
+      <c r="E4" s="8" t="s">
+        <v>83</v>
       </c>
       <c r="F4" t="s">
-        <v>12</v>
-      </c>
-      <c r="G4" s="11" t="s">
-        <v>12</v>
+        <v>11</v>
+      </c>
+      <c r="G4" s="8" t="s">
+        <v>11</v>
       </c>
       <c r="H4">
         <v>0.09</v>
@@ -888,7 +888,7 @@
       <c r="I4">
         <v>0</v>
       </c>
-      <c r="J4" s="11">
+      <c r="J4" s="8">
         <v>0</v>
       </c>
       <c r="K4">
@@ -909,16 +909,16 @@
         <v>6</v>
       </c>
       <c r="D5" t="s">
-        <v>83</v>
-      </c>
-      <c r="E5" s="11" t="s">
-        <v>84</v>
+        <v>82</v>
+      </c>
+      <c r="E5" s="8" t="s">
+        <v>83</v>
       </c>
       <c r="F5" t="s">
+        <v>12</v>
+      </c>
+      <c r="G5" s="8" t="s">
         <v>13</v>
-      </c>
-      <c r="G5" s="11" t="s">
-        <v>14</v>
       </c>
       <c r="H5">
         <v>0.53</v>
@@ -926,7 +926,7 @@
       <c r="I5">
         <v>0</v>
       </c>
-      <c r="J5" s="11">
+      <c r="J5" s="8">
         <v>0.08</v>
       </c>
       <c r="K5">
@@ -947,16 +947,16 @@
         <v>8</v>
       </c>
       <c r="D6" t="s">
-        <v>83</v>
-      </c>
-      <c r="E6" s="11" t="s">
-        <v>84</v>
+        <v>82</v>
+      </c>
+      <c r="E6" s="8" t="s">
+        <v>83</v>
       </c>
       <c r="F6" t="s">
+        <v>14</v>
+      </c>
+      <c r="G6" s="8" t="s">
         <v>15</v>
-      </c>
-      <c r="G6" s="11" t="s">
-        <v>16</v>
       </c>
       <c r="H6">
         <v>0.85</v>
@@ -964,7 +964,7 @@
       <c r="I6">
         <v>0.82</v>
       </c>
-      <c r="J6" s="11">
+      <c r="J6" s="8">
         <v>0.85</v>
       </c>
       <c r="K6">
@@ -985,16 +985,16 @@
         <v>10</v>
       </c>
       <c r="D7" t="s">
-        <v>83</v>
-      </c>
-      <c r="E7" s="11" t="s">
-        <v>84</v>
+        <v>82</v>
+      </c>
+      <c r="E7" s="8" t="s">
+        <v>83</v>
       </c>
       <c r="F7" t="s">
-        <v>17</v>
-      </c>
-      <c r="G7" s="11" t="s">
-        <v>17</v>
+        <v>16</v>
+      </c>
+      <c r="G7" s="8" t="s">
+        <v>16</v>
       </c>
       <c r="H7">
         <v>0.97</v>
@@ -1002,7 +1002,7 @@
       <c r="I7">
         <v>0.97</v>
       </c>
-      <c r="J7" s="11">
+      <c r="J7" s="8">
         <v>0.97</v>
       </c>
       <c r="K7">
@@ -1023,16 +1023,16 @@
         <v>2</v>
       </c>
       <c r="D8" t="s">
-        <v>82</v>
-      </c>
-      <c r="E8" s="11" t="s">
-        <v>84</v>
+        <v>81</v>
+      </c>
+      <c r="E8" s="8" t="s">
+        <v>83</v>
       </c>
       <c r="F8" t="s">
-        <v>13</v>
-      </c>
-      <c r="G8" s="11" t="s">
-        <v>13</v>
+        <v>12</v>
+      </c>
+      <c r="G8" s="8" t="s">
+        <v>12</v>
       </c>
       <c r="H8">
         <v>0</v>
@@ -1040,7 +1040,7 @@
       <c r="I8">
         <v>0</v>
       </c>
-      <c r="J8" s="11">
+      <c r="J8" s="8">
         <v>0</v>
       </c>
       <c r="K8">
@@ -1061,16 +1061,16 @@
         <v>4</v>
       </c>
       <c r="D9" t="s">
-        <v>82</v>
-      </c>
-      <c r="E9" s="11" t="s">
-        <v>84</v>
+        <v>81</v>
+      </c>
+      <c r="E9" s="8" t="s">
+        <v>83</v>
       </c>
       <c r="F9" t="s">
-        <v>18</v>
-      </c>
-      <c r="G9" s="11" t="s">
-        <v>18</v>
+        <v>17</v>
+      </c>
+      <c r="G9" s="8" t="s">
+        <v>17</v>
       </c>
       <c r="H9">
         <v>0.03</v>
@@ -1078,7 +1078,7 @@
       <c r="I9">
         <v>0</v>
       </c>
-      <c r="J9" s="11">
+      <c r="J9" s="8">
         <v>0</v>
       </c>
       <c r="K9">
@@ -1099,16 +1099,16 @@
         <v>6</v>
       </c>
       <c r="D10" t="s">
-        <v>82</v>
-      </c>
-      <c r="E10" s="11" t="s">
-        <v>84</v>
+        <v>81</v>
+      </c>
+      <c r="E10" s="8" t="s">
+        <v>83</v>
       </c>
       <c r="F10" t="s">
-        <v>19</v>
-      </c>
-      <c r="G10" s="11" t="s">
-        <v>19</v>
+        <v>18</v>
+      </c>
+      <c r="G10" s="8" t="s">
+        <v>18</v>
       </c>
       <c r="H10">
         <v>0.27</v>
@@ -1116,7 +1116,7 @@
       <c r="I10">
         <v>0</v>
       </c>
-      <c r="J10" s="11">
+      <c r="J10" s="8">
         <v>0</v>
       </c>
       <c r="K10">
@@ -1137,16 +1137,16 @@
         <v>8</v>
       </c>
       <c r="D11" t="s">
-        <v>82</v>
-      </c>
-      <c r="E11" s="11" t="s">
-        <v>84</v>
+        <v>81</v>
+      </c>
+      <c r="E11" s="8" t="s">
+        <v>83</v>
       </c>
       <c r="F11" t="s">
+        <v>19</v>
+      </c>
+      <c r="G11" s="8" t="s">
         <v>20</v>
-      </c>
-      <c r="G11" s="11" t="s">
-        <v>21</v>
       </c>
       <c r="H11">
         <v>0.64</v>
@@ -1154,7 +1154,7 @@
       <c r="I11">
         <v>0.1</v>
       </c>
-      <c r="J11" s="11">
+      <c r="J11" s="8">
         <v>0.12</v>
       </c>
       <c r="K11">
@@ -1175,16 +1175,16 @@
         <v>10</v>
       </c>
       <c r="D12" t="s">
-        <v>82</v>
-      </c>
-      <c r="E12" s="11" t="s">
-        <v>84</v>
+        <v>81</v>
+      </c>
+      <c r="E12" s="8" t="s">
+        <v>83</v>
       </c>
       <c r="F12" t="s">
+        <v>21</v>
+      </c>
+      <c r="G12" s="8" t="s">
         <v>22</v>
-      </c>
-      <c r="G12" s="11" t="s">
-        <v>23</v>
       </c>
       <c r="H12">
         <v>0.87</v>
@@ -1192,7 +1192,7 @@
       <c r="I12">
         <v>0.83</v>
       </c>
-      <c r="J12" s="11">
+      <c r="J12" s="8">
         <v>0.85</v>
       </c>
       <c r="K12">
@@ -1213,24 +1213,24 @@
         <v>2</v>
       </c>
       <c r="D13" t="s">
-        <v>81</v>
-      </c>
-      <c r="E13" s="11" t="s">
-        <v>84</v>
+        <v>80</v>
+      </c>
+      <c r="E13" s="8" t="s">
+        <v>83</v>
       </c>
       <c r="F13" t="s">
+        <v>23</v>
+      </c>
+      <c r="G13" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="G13" s="11" t="s">
-        <v>25</v>
-      </c>
       <c r="H13">
         <v>0</v>
       </c>
       <c r="I13">
         <v>0</v>
       </c>
-      <c r="J13" s="11">
+      <c r="J13" s="8">
         <v>0</v>
       </c>
       <c r="K13">
@@ -1251,24 +1251,24 @@
         <v>4</v>
       </c>
       <c r="D14" t="s">
-        <v>81</v>
-      </c>
-      <c r="E14" s="11" t="s">
-        <v>84</v>
+        <v>80</v>
+      </c>
+      <c r="E14" s="8" t="s">
+        <v>83</v>
       </c>
       <c r="F14" t="s">
+        <v>25</v>
+      </c>
+      <c r="G14" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="G14" s="11" t="s">
-        <v>27</v>
-      </c>
       <c r="H14">
         <v>0</v>
       </c>
       <c r="I14">
         <v>0</v>
       </c>
-      <c r="J14" s="11">
+      <c r="J14" s="8">
         <v>0</v>
       </c>
       <c r="K14">
@@ -1289,24 +1289,24 @@
         <v>6</v>
       </c>
       <c r="D15" t="s">
-        <v>81</v>
-      </c>
-      <c r="E15" s="11" t="s">
-        <v>84</v>
+        <v>80</v>
+      </c>
+      <c r="E15" s="8" t="s">
+        <v>83</v>
       </c>
       <c r="F15" t="s">
+        <v>27</v>
+      </c>
+      <c r="G15" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="G15" s="11" t="s">
-        <v>29</v>
-      </c>
       <c r="H15">
         <v>0</v>
       </c>
       <c r="I15">
         <v>0</v>
       </c>
-      <c r="J15" s="11">
+      <c r="J15" s="8">
         <v>0</v>
       </c>
       <c r="K15">
@@ -1327,24 +1327,24 @@
         <v>8</v>
       </c>
       <c r="D16" t="s">
-        <v>81</v>
-      </c>
-      <c r="E16" s="11" t="s">
-        <v>84</v>
+        <v>80</v>
+      </c>
+      <c r="E16" s="8" t="s">
+        <v>83</v>
       </c>
       <c r="F16" t="s">
+        <v>29</v>
+      </c>
+      <c r="G16" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="G16" s="11" t="s">
-        <v>31</v>
-      </c>
       <c r="H16">
         <v>0</v>
       </c>
       <c r="I16">
         <v>0</v>
       </c>
-      <c r="J16" s="11">
+      <c r="J16" s="8">
         <v>0</v>
       </c>
       <c r="K16">
@@ -1365,16 +1365,16 @@
         <v>10</v>
       </c>
       <c r="D17" t="s">
-        <v>81</v>
-      </c>
-      <c r="E17" s="11" t="s">
-        <v>84</v>
+        <v>80</v>
+      </c>
+      <c r="E17" s="8" t="s">
+        <v>83</v>
       </c>
       <c r="F17" t="s">
+        <v>31</v>
+      </c>
+      <c r="G17" s="8" t="s">
         <v>32</v>
-      </c>
-      <c r="G17" s="11" t="s">
-        <v>33</v>
       </c>
       <c r="H17">
         <v>7.0000000000000007E-2</v>
@@ -1382,7 +1382,7 @@
       <c r="I17">
         <v>0</v>
       </c>
-      <c r="J17" s="11">
+      <c r="J17" s="8">
         <v>0</v>
       </c>
       <c r="K17">
@@ -1403,16 +1403,16 @@
         <v>2</v>
       </c>
       <c r="D18" t="s">
-        <v>83</v>
-      </c>
-      <c r="E18" s="11" t="s">
-        <v>84</v>
+        <v>82</v>
+      </c>
+      <c r="E18" s="8" t="s">
+        <v>83</v>
       </c>
       <c r="F18" t="s">
-        <v>12</v>
-      </c>
-      <c r="G18" s="11" t="s">
-        <v>12</v>
+        <v>11</v>
+      </c>
+      <c r="G18" s="8" t="s">
+        <v>11</v>
       </c>
       <c r="H18">
         <v>0.03</v>
@@ -1420,7 +1420,7 @@
       <c r="I18">
         <v>0</v>
       </c>
-      <c r="J18" s="11">
+      <c r="J18" s="8">
         <v>0</v>
       </c>
       <c r="K18">
@@ -1441,16 +1441,16 @@
         <v>4</v>
       </c>
       <c r="D19" t="s">
-        <v>83</v>
-      </c>
-      <c r="E19" s="11" t="s">
-        <v>84</v>
+        <v>82</v>
+      </c>
+      <c r="E19" s="8" t="s">
+        <v>83</v>
       </c>
       <c r="F19" t="s">
-        <v>12</v>
-      </c>
-      <c r="G19" s="11" t="s">
-        <v>34</v>
+        <v>11</v>
+      </c>
+      <c r="G19" s="8" t="s">
+        <v>33</v>
       </c>
       <c r="H19">
         <v>0.12</v>
@@ -1458,7 +1458,7 @@
       <c r="I19">
         <v>0</v>
       </c>
-      <c r="J19" s="11">
+      <c r="J19" s="8">
         <v>0</v>
       </c>
       <c r="K19">
@@ -1479,16 +1479,16 @@
         <v>6</v>
       </c>
       <c r="D20" t="s">
-        <v>83</v>
-      </c>
-      <c r="E20" s="11" t="s">
-        <v>84</v>
+        <v>82</v>
+      </c>
+      <c r="E20" s="8" t="s">
+        <v>83</v>
       </c>
       <c r="F20" t="s">
+        <v>34</v>
+      </c>
+      <c r="G20" s="8" t="s">
         <v>35</v>
-      </c>
-      <c r="G20" s="11" t="s">
-        <v>36</v>
       </c>
       <c r="H20">
         <v>0.27</v>
@@ -1496,7 +1496,7 @@
       <c r="I20">
         <v>0</v>
       </c>
-      <c r="J20" s="11">
+      <c r="J20" s="8">
         <v>0.01</v>
       </c>
       <c r="K20">
@@ -1517,16 +1517,16 @@
         <v>8</v>
       </c>
       <c r="D21" t="s">
-        <v>83</v>
-      </c>
-      <c r="E21" s="11" t="s">
-        <v>84</v>
+        <v>82</v>
+      </c>
+      <c r="E21" s="8" t="s">
+        <v>83</v>
       </c>
       <c r="F21" t="s">
+        <v>36</v>
+      </c>
+      <c r="G21" s="8" t="s">
         <v>37</v>
-      </c>
-      <c r="G21" s="11" t="s">
-        <v>38</v>
       </c>
       <c r="H21">
         <v>0.44</v>
@@ -1534,7 +1534,7 @@
       <c r="I21">
         <v>0.04</v>
       </c>
-      <c r="J21" s="11">
+      <c r="J21" s="8">
         <v>0.04</v>
       </c>
       <c r="K21">
@@ -1555,16 +1555,16 @@
         <v>10</v>
       </c>
       <c r="D22" t="s">
-        <v>83</v>
-      </c>
-      <c r="E22" s="11" t="s">
-        <v>84</v>
+        <v>82</v>
+      </c>
+      <c r="E22" s="8" t="s">
+        <v>83</v>
       </c>
       <c r="F22" t="s">
+        <v>38</v>
+      </c>
+      <c r="G22" s="8" t="s">
         <v>39</v>
-      </c>
-      <c r="G22" s="11" t="s">
-        <v>40</v>
       </c>
       <c r="H22">
         <v>0.62</v>
@@ -1572,7 +1572,7 @@
       <c r="I22">
         <v>0.23</v>
       </c>
-      <c r="J22" s="11">
+      <c r="J22" s="8">
         <v>0.28000000000000003</v>
       </c>
       <c r="K22">
@@ -1593,16 +1593,16 @@
         <v>2</v>
       </c>
       <c r="D23" t="s">
-        <v>82</v>
-      </c>
-      <c r="E23" s="11" t="s">
-        <v>84</v>
+        <v>81</v>
+      </c>
+      <c r="E23" s="8" t="s">
+        <v>83</v>
       </c>
       <c r="F23" t="s">
-        <v>34</v>
-      </c>
-      <c r="G23" s="11" t="s">
-        <v>34</v>
+        <v>33</v>
+      </c>
+      <c r="G23" s="8" t="s">
+        <v>33</v>
       </c>
       <c r="H23">
         <v>0.02</v>
@@ -1610,7 +1610,7 @@
       <c r="I23">
         <v>0</v>
       </c>
-      <c r="J23" s="11">
+      <c r="J23" s="8">
         <v>0</v>
       </c>
       <c r="K23">
@@ -1631,16 +1631,16 @@
         <v>4</v>
       </c>
       <c r="D24" t="s">
-        <v>82</v>
-      </c>
-      <c r="E24" s="11" t="s">
-        <v>84</v>
+        <v>81</v>
+      </c>
+      <c r="E24" s="8" t="s">
+        <v>83</v>
       </c>
       <c r="F24" t="s">
-        <v>19</v>
-      </c>
-      <c r="G24" s="11" t="s">
-        <v>19</v>
+        <v>18</v>
+      </c>
+      <c r="G24" s="8" t="s">
+        <v>18</v>
       </c>
       <c r="H24">
         <v>0.08</v>
@@ -1648,7 +1648,7 @@
       <c r="I24">
         <v>0</v>
       </c>
-      <c r="J24" s="11">
+      <c r="J24" s="8">
         <v>0</v>
       </c>
       <c r="K24">
@@ -1669,16 +1669,16 @@
         <v>6</v>
       </c>
       <c r="D25" t="s">
-        <v>82</v>
-      </c>
-      <c r="E25" s="11" t="s">
-        <v>84</v>
+        <v>81</v>
+      </c>
+      <c r="E25" s="8" t="s">
+        <v>83</v>
       </c>
       <c r="F25" t="s">
-        <v>13</v>
-      </c>
-      <c r="G25" s="11" t="s">
-        <v>13</v>
+        <v>12</v>
+      </c>
+      <c r="G25" s="8" t="s">
+        <v>12</v>
       </c>
       <c r="H25">
         <v>0.19</v>
@@ -1686,7 +1686,7 @@
       <c r="I25">
         <v>0</v>
       </c>
-      <c r="J25" s="11">
+      <c r="J25" s="8">
         <v>0</v>
       </c>
       <c r="K25">
@@ -1707,16 +1707,16 @@
         <v>8</v>
       </c>
       <c r="D26" t="s">
-        <v>82</v>
-      </c>
-      <c r="E26" s="11" t="s">
-        <v>84</v>
+        <v>81</v>
+      </c>
+      <c r="E26" s="8" t="s">
+        <v>83</v>
       </c>
       <c r="F26" t="s">
-        <v>13</v>
-      </c>
-      <c r="G26" s="11" t="s">
-        <v>35</v>
+        <v>12</v>
+      </c>
+      <c r="G26" s="8" t="s">
+        <v>34</v>
       </c>
       <c r="H26">
         <v>0.34</v>
@@ -1724,7 +1724,7 @@
       <c r="I26">
         <v>0</v>
       </c>
-      <c r="J26" s="11">
+      <c r="J26" s="8">
         <v>0</v>
       </c>
       <c r="K26">
@@ -1745,16 +1745,16 @@
         <v>10</v>
       </c>
       <c r="D27" t="s">
-        <v>82</v>
-      </c>
-      <c r="E27" s="11" t="s">
-        <v>84</v>
+        <v>81</v>
+      </c>
+      <c r="E27" s="8" t="s">
+        <v>83</v>
       </c>
       <c r="F27" t="s">
+        <v>40</v>
+      </c>
+      <c r="G27" s="8" t="s">
         <v>41</v>
-      </c>
-      <c r="G27" s="11" t="s">
-        <v>42</v>
       </c>
       <c r="H27">
         <v>0.51</v>
@@ -1762,7 +1762,7 @@
       <c r="I27">
         <v>0.02</v>
       </c>
-      <c r="J27" s="11">
+      <c r="J27" s="8">
         <v>0.03</v>
       </c>
       <c r="K27">
@@ -1783,24 +1783,24 @@
         <v>2</v>
       </c>
       <c r="D28" t="s">
-        <v>81</v>
-      </c>
-      <c r="E28" s="11" t="s">
-        <v>84</v>
+        <v>80</v>
+      </c>
+      <c r="E28" s="8" t="s">
+        <v>83</v>
       </c>
       <c r="F28" t="s">
+        <v>42</v>
+      </c>
+      <c r="G28" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="G28" s="11" t="s">
-        <v>44</v>
-      </c>
       <c r="H28">
         <v>0</v>
       </c>
       <c r="I28">
         <v>0</v>
       </c>
-      <c r="J28" s="11">
+      <c r="J28" s="8">
         <v>0</v>
       </c>
       <c r="K28">
@@ -1821,24 +1821,24 @@
         <v>4</v>
       </c>
       <c r="D29" t="s">
-        <v>81</v>
-      </c>
-      <c r="E29" s="11" t="s">
-        <v>84</v>
+        <v>80</v>
+      </c>
+      <c r="E29" s="8" t="s">
+        <v>83</v>
       </c>
       <c r="F29" t="s">
+        <v>44</v>
+      </c>
+      <c r="G29" s="8" t="s">
         <v>45</v>
       </c>
-      <c r="G29" s="11" t="s">
-        <v>46</v>
-      </c>
       <c r="H29">
         <v>0</v>
       </c>
       <c r="I29">
         <v>0</v>
       </c>
-      <c r="J29" s="11">
+      <c r="J29" s="8">
         <v>0</v>
       </c>
       <c r="K29">
@@ -1859,16 +1859,16 @@
         <v>6</v>
       </c>
       <c r="D30" t="s">
-        <v>81</v>
-      </c>
-      <c r="E30" s="11" t="s">
-        <v>84</v>
+        <v>80</v>
+      </c>
+      <c r="E30" s="8" t="s">
+        <v>83</v>
       </c>
       <c r="F30" t="s">
+        <v>46</v>
+      </c>
+      <c r="G30" s="8" t="s">
         <v>47</v>
-      </c>
-      <c r="G30" s="11" t="s">
-        <v>48</v>
       </c>
       <c r="H30">
         <v>0.01</v>
@@ -1876,7 +1876,7 @@
       <c r="I30">
         <v>0</v>
       </c>
-      <c r="J30" s="11">
+      <c r="J30" s="8">
         <v>0</v>
       </c>
       <c r="K30">
@@ -1897,16 +1897,16 @@
         <v>8</v>
       </c>
       <c r="D31" t="s">
-        <v>81</v>
-      </c>
-      <c r="E31" s="11" t="s">
-        <v>84</v>
+        <v>80</v>
+      </c>
+      <c r="E31" s="8" t="s">
+        <v>83</v>
       </c>
       <c r="F31" t="s">
+        <v>48</v>
+      </c>
+      <c r="G31" s="8" t="s">
         <v>49</v>
-      </c>
-      <c r="G31" s="11" t="s">
-        <v>50</v>
       </c>
       <c r="H31">
         <v>0.03</v>
@@ -1914,7 +1914,7 @@
       <c r="I31">
         <v>0</v>
       </c>
-      <c r="J31" s="11">
+      <c r="J31" s="8">
         <v>0</v>
       </c>
       <c r="K31">
@@ -1935,16 +1935,16 @@
         <v>10</v>
       </c>
       <c r="D32" t="s">
-        <v>81</v>
-      </c>
-      <c r="E32" s="11" t="s">
-        <v>84</v>
+        <v>80</v>
+      </c>
+      <c r="E32" s="8" t="s">
+        <v>83</v>
       </c>
       <c r="F32" t="s">
+        <v>50</v>
+      </c>
+      <c r="G32" s="8" t="s">
         <v>51</v>
-      </c>
-      <c r="G32" s="11" t="s">
-        <v>52</v>
       </c>
       <c r="H32">
         <v>0.11</v>
@@ -1952,7 +1952,7 @@
       <c r="I32">
         <v>0</v>
       </c>
-      <c r="J32" s="11">
+      <c r="J32" s="8">
         <v>0</v>
       </c>
       <c r="K32">
@@ -1973,16 +1973,16 @@
         <v>2</v>
       </c>
       <c r="D33" t="s">
-        <v>83</v>
-      </c>
-      <c r="E33" s="11" t="s">
-        <v>84</v>
+        <v>82</v>
+      </c>
+      <c r="E33" s="8" t="s">
+        <v>83</v>
       </c>
       <c r="F33" t="s">
-        <v>12</v>
-      </c>
-      <c r="G33" s="11" t="s">
-        <v>19</v>
+        <v>11</v>
+      </c>
+      <c r="G33" s="8" t="s">
+        <v>18</v>
       </c>
       <c r="H33">
         <v>0.01</v>
@@ -1990,7 +1990,7 @@
       <c r="I33">
         <v>0</v>
       </c>
-      <c r="J33" s="11">
+      <c r="J33" s="8">
         <v>0</v>
       </c>
       <c r="K33">
@@ -2011,16 +2011,16 @@
         <v>4</v>
       </c>
       <c r="D34" t="s">
-        <v>83</v>
-      </c>
-      <c r="E34" s="11" t="s">
-        <v>84</v>
+        <v>82</v>
+      </c>
+      <c r="E34" s="8" t="s">
+        <v>83</v>
       </c>
       <c r="F34" t="s">
-        <v>12</v>
-      </c>
-      <c r="G34" s="11" t="s">
-        <v>19</v>
+        <v>11</v>
+      </c>
+      <c r="G34" s="8" t="s">
+        <v>18</v>
       </c>
       <c r="H34">
         <v>0.04</v>
@@ -2028,7 +2028,7 @@
       <c r="I34">
         <v>0</v>
       </c>
-      <c r="J34" s="11">
+      <c r="J34" s="8">
         <v>0</v>
       </c>
       <c r="K34">
@@ -2049,16 +2049,16 @@
         <v>6</v>
       </c>
       <c r="D35" t="s">
-        <v>83</v>
-      </c>
-      <c r="E35" s="11" t="s">
-        <v>84</v>
+        <v>82</v>
+      </c>
+      <c r="E35" s="8" t="s">
+        <v>83</v>
       </c>
       <c r="F35" t="s">
-        <v>12</v>
-      </c>
-      <c r="G35" s="11" t="s">
-        <v>19</v>
+        <v>11</v>
+      </c>
+      <c r="G35" s="8" t="s">
+        <v>18</v>
       </c>
       <c r="H35">
         <v>0.09</v>
@@ -2066,7 +2066,7 @@
       <c r="I35">
         <v>0</v>
       </c>
-      <c r="J35" s="11">
+      <c r="J35" s="8">
         <v>0</v>
       </c>
       <c r="K35">
@@ -2087,16 +2087,16 @@
         <v>8</v>
       </c>
       <c r="D36" t="s">
-        <v>83</v>
-      </c>
-      <c r="E36" s="11" t="s">
-        <v>84</v>
+        <v>82</v>
+      </c>
+      <c r="E36" s="8" t="s">
+        <v>83</v>
       </c>
       <c r="F36" t="s">
-        <v>12</v>
-      </c>
-      <c r="G36" s="11" t="s">
-        <v>19</v>
+        <v>11</v>
+      </c>
+      <c r="G36" s="8" t="s">
+        <v>18</v>
       </c>
       <c r="H36">
         <v>0.15</v>
@@ -2104,7 +2104,7 @@
       <c r="I36">
         <v>0</v>
       </c>
-      <c r="J36" s="11">
+      <c r="J36" s="8">
         <v>0</v>
       </c>
       <c r="K36">
@@ -2125,16 +2125,16 @@
         <v>10</v>
       </c>
       <c r="D37" t="s">
-        <v>83</v>
-      </c>
-      <c r="E37" s="11" t="s">
-        <v>84</v>
+        <v>82</v>
+      </c>
+      <c r="E37" s="8" t="s">
+        <v>83</v>
       </c>
       <c r="F37" t="s">
-        <v>12</v>
-      </c>
-      <c r="G37" s="11" t="s">
-        <v>35</v>
+        <v>11</v>
+      </c>
+      <c r="G37" s="8" t="s">
+        <v>34</v>
       </c>
       <c r="H37">
         <v>0.21</v>
@@ -2142,7 +2142,7 @@
       <c r="I37">
         <v>0</v>
       </c>
-      <c r="J37" s="11">
+      <c r="J37" s="8">
         <v>0</v>
       </c>
       <c r="K37">
@@ -2163,16 +2163,16 @@
         <v>2</v>
       </c>
       <c r="D38" t="s">
-        <v>82</v>
-      </c>
-      <c r="E38" s="11" t="s">
-        <v>84</v>
+        <v>81</v>
+      </c>
+      <c r="E38" s="8" t="s">
+        <v>83</v>
       </c>
       <c r="F38" t="s">
-        <v>12</v>
-      </c>
-      <c r="G38" s="11" t="s">
-        <v>12</v>
+        <v>11</v>
+      </c>
+      <c r="G38" s="8" t="s">
+        <v>11</v>
       </c>
       <c r="H38">
         <v>0.01</v>
@@ -2180,7 +2180,7 @@
       <c r="I38">
         <v>0</v>
       </c>
-      <c r="J38" s="11">
+      <c r="J38" s="8">
         <v>0</v>
       </c>
       <c r="K38">
@@ -2201,16 +2201,16 @@
         <v>4</v>
       </c>
       <c r="D39" t="s">
-        <v>82</v>
-      </c>
-      <c r="E39" s="11" t="s">
-        <v>84</v>
+        <v>81</v>
+      </c>
+      <c r="E39" s="8" t="s">
+        <v>83</v>
       </c>
       <c r="F39" t="s">
-        <v>12</v>
-      </c>
-      <c r="G39" s="11" t="s">
-        <v>12</v>
+        <v>11</v>
+      </c>
+      <c r="G39" s="8" t="s">
+        <v>11</v>
       </c>
       <c r="H39">
         <v>0.03</v>
@@ -2218,7 +2218,7 @@
       <c r="I39">
         <v>0</v>
       </c>
-      <c r="J39" s="11">
+      <c r="J39" s="8">
         <v>0</v>
       </c>
       <c r="K39">
@@ -2239,16 +2239,16 @@
         <v>6</v>
       </c>
       <c r="D40" t="s">
-        <v>82</v>
-      </c>
-      <c r="E40" s="11" t="s">
-        <v>84</v>
+        <v>81</v>
+      </c>
+      <c r="E40" s="8" t="s">
+        <v>83</v>
       </c>
       <c r="F40" t="s">
-        <v>12</v>
-      </c>
-      <c r="G40" s="11" t="s">
-        <v>12</v>
+        <v>11</v>
+      </c>
+      <c r="G40" s="8" t="s">
+        <v>11</v>
       </c>
       <c r="H40">
         <v>7.0000000000000007E-2</v>
@@ -2256,7 +2256,7 @@
       <c r="I40">
         <v>0</v>
       </c>
-      <c r="J40" s="11">
+      <c r="J40" s="8">
         <v>0</v>
       </c>
       <c r="K40">
@@ -2277,16 +2277,16 @@
         <v>8</v>
       </c>
       <c r="D41" t="s">
-        <v>82</v>
-      </c>
-      <c r="E41" s="11" t="s">
-        <v>84</v>
+        <v>81</v>
+      </c>
+      <c r="E41" s="8" t="s">
+        <v>83</v>
       </c>
       <c r="F41" t="s">
-        <v>12</v>
-      </c>
-      <c r="G41" s="11" t="s">
-        <v>12</v>
+        <v>11</v>
+      </c>
+      <c r="G41" s="8" t="s">
+        <v>11</v>
       </c>
       <c r="H41">
         <v>0.11</v>
@@ -2294,7 +2294,7 @@
       <c r="I41">
         <v>0</v>
       </c>
-      <c r="J41" s="11">
+      <c r="J41" s="8">
         <v>0</v>
       </c>
       <c r="K41">
@@ -2315,16 +2315,16 @@
         <v>10</v>
       </c>
       <c r="D42" t="s">
-        <v>82</v>
-      </c>
-      <c r="E42" s="11" t="s">
-        <v>84</v>
+        <v>81</v>
+      </c>
+      <c r="E42" s="8" t="s">
+        <v>83</v>
       </c>
       <c r="F42" t="s">
-        <v>12</v>
-      </c>
-      <c r="G42" s="11" t="s">
-        <v>12</v>
+        <v>11</v>
+      </c>
+      <c r="G42" s="8" t="s">
+        <v>11</v>
       </c>
       <c r="H42">
         <v>0.17</v>
@@ -2332,7 +2332,7 @@
       <c r="I42">
         <v>0</v>
       </c>
-      <c r="J42" s="11">
+      <c r="J42" s="8">
         <v>0</v>
       </c>
       <c r="K42">
@@ -2353,24 +2353,24 @@
         <v>2</v>
       </c>
       <c r="D43" t="s">
-        <v>81</v>
-      </c>
-      <c r="E43" s="11" t="s">
-        <v>84</v>
+        <v>80</v>
+      </c>
+      <c r="E43" s="8" t="s">
+        <v>83</v>
       </c>
       <c r="F43" t="s">
+        <v>52</v>
+      </c>
+      <c r="G43" s="8" t="s">
         <v>53</v>
       </c>
-      <c r="G43" s="11" t="s">
-        <v>54</v>
-      </c>
       <c r="H43">
         <v>0</v>
       </c>
       <c r="I43">
         <v>0</v>
       </c>
-      <c r="J43" s="11">
+      <c r="J43" s="8">
         <v>0</v>
       </c>
       <c r="K43">
@@ -2391,16 +2391,16 @@
         <v>4</v>
       </c>
       <c r="D44" t="s">
-        <v>81</v>
-      </c>
-      <c r="E44" s="11" t="s">
-        <v>84</v>
+        <v>80</v>
+      </c>
+      <c r="E44" s="8" t="s">
+        <v>83</v>
       </c>
       <c r="F44" t="s">
+        <v>54</v>
+      </c>
+      <c r="G44" s="8" t="s">
         <v>55</v>
-      </c>
-      <c r="G44" s="11" t="s">
-        <v>56</v>
       </c>
       <c r="H44">
         <v>0.01</v>
@@ -2408,7 +2408,7 @@
       <c r="I44">
         <v>0</v>
       </c>
-      <c r="J44" s="11">
+      <c r="J44" s="8">
         <v>0</v>
       </c>
       <c r="K44">
@@ -2429,16 +2429,16 @@
         <v>6</v>
       </c>
       <c r="D45" t="s">
-        <v>81</v>
-      </c>
-      <c r="E45" s="11" t="s">
-        <v>84</v>
+        <v>80</v>
+      </c>
+      <c r="E45" s="8" t="s">
+        <v>83</v>
       </c>
       <c r="F45" t="s">
+        <v>56</v>
+      </c>
+      <c r="G45" s="8" t="s">
         <v>57</v>
-      </c>
-      <c r="G45" s="11" t="s">
-        <v>58</v>
       </c>
       <c r="H45">
         <v>0.03</v>
@@ -2446,7 +2446,7 @@
       <c r="I45">
         <v>0</v>
       </c>
-      <c r="J45" s="11">
+      <c r="J45" s="8">
         <v>0</v>
       </c>
       <c r="K45">
@@ -2467,16 +2467,16 @@
         <v>8</v>
       </c>
       <c r="D46" t="s">
-        <v>81</v>
-      </c>
-      <c r="E46" s="11" t="s">
-        <v>84</v>
+        <v>80</v>
+      </c>
+      <c r="E46" s="8" t="s">
+        <v>83</v>
       </c>
       <c r="F46" t="s">
+        <v>58</v>
+      </c>
+      <c r="G46" s="8" t="s">
         <v>59</v>
-      </c>
-      <c r="G46" s="11" t="s">
-        <v>60</v>
       </c>
       <c r="H46">
         <v>0.05</v>
@@ -2484,7 +2484,7 @@
       <c r="I46">
         <v>0</v>
       </c>
-      <c r="J46" s="11">
+      <c r="J46" s="8">
         <v>0</v>
       </c>
       <c r="K46">
@@ -2505,16 +2505,16 @@
         <v>10</v>
       </c>
       <c r="D47" t="s">
-        <v>81</v>
-      </c>
-      <c r="E47" s="11" t="s">
-        <v>84</v>
+        <v>80</v>
+      </c>
+      <c r="E47" s="8" t="s">
+        <v>83</v>
       </c>
       <c r="F47" t="s">
+        <v>60</v>
+      </c>
+      <c r="G47" s="8" t="s">
         <v>61</v>
-      </c>
-      <c r="G47" s="11" t="s">
-        <v>62</v>
       </c>
       <c r="H47">
         <v>0.09</v>
@@ -2522,7 +2522,7 @@
       <c r="I47">
         <v>0</v>
       </c>
-      <c r="J47" s="11">
+      <c r="J47" s="8">
         <v>0</v>
       </c>
       <c r="K47">
@@ -2543,16 +2543,16 @@
         <v>2</v>
       </c>
       <c r="D48" t="s">
-        <v>83</v>
-      </c>
-      <c r="E48" s="11" t="s">
-        <v>84</v>
+        <v>82</v>
+      </c>
+      <c r="E48" s="8" t="s">
+        <v>83</v>
       </c>
       <c r="F48" t="s">
-        <v>19</v>
-      </c>
-      <c r="G48" s="11" t="s">
-        <v>13</v>
+        <v>18</v>
+      </c>
+      <c r="G48" s="8" t="s">
+        <v>12</v>
       </c>
       <c r="H48">
         <v>0.01</v>
@@ -2560,7 +2560,7 @@
       <c r="I48">
         <v>0</v>
       </c>
-      <c r="J48" s="11">
+      <c r="J48" s="8">
         <v>0</v>
       </c>
       <c r="K48">
@@ -2581,16 +2581,16 @@
         <v>4</v>
       </c>
       <c r="D49" t="s">
-        <v>83</v>
-      </c>
-      <c r="E49" s="11" t="s">
-        <v>84</v>
+        <v>82</v>
+      </c>
+      <c r="E49" s="8" t="s">
+        <v>83</v>
       </c>
       <c r="F49" t="s">
-        <v>12</v>
-      </c>
-      <c r="G49" s="11" t="s">
-        <v>19</v>
+        <v>11</v>
+      </c>
+      <c r="G49" s="8" t="s">
+        <v>18</v>
       </c>
       <c r="H49">
         <v>0.02</v>
@@ -2598,7 +2598,7 @@
       <c r="I49">
         <v>0</v>
       </c>
-      <c r="J49" s="11">
+      <c r="J49" s="8">
         <v>0</v>
       </c>
       <c r="K49">
@@ -2619,16 +2619,16 @@
         <v>6</v>
       </c>
       <c r="D50" t="s">
-        <v>83</v>
-      </c>
-      <c r="E50" s="11" t="s">
-        <v>84</v>
+        <v>82</v>
+      </c>
+      <c r="E50" s="8" t="s">
+        <v>83</v>
       </c>
       <c r="F50" t="s">
-        <v>12</v>
-      </c>
-      <c r="G50" s="11" t="s">
-        <v>19</v>
+        <v>11</v>
+      </c>
+      <c r="G50" s="8" t="s">
+        <v>18</v>
       </c>
       <c r="H50">
         <v>0.05</v>
@@ -2636,7 +2636,7 @@
       <c r="I50">
         <v>0</v>
       </c>
-      <c r="J50" s="11">
+      <c r="J50" s="8">
         <v>0</v>
       </c>
       <c r="K50">
@@ -2657,16 +2657,16 @@
         <v>8</v>
       </c>
       <c r="D51" t="s">
-        <v>83</v>
-      </c>
-      <c r="E51" s="11" t="s">
-        <v>84</v>
+        <v>82</v>
+      </c>
+      <c r="E51" s="8" t="s">
+        <v>83</v>
       </c>
       <c r="F51" t="s">
-        <v>12</v>
-      </c>
-      <c r="G51" s="11" t="s">
-        <v>19</v>
+        <v>11</v>
+      </c>
+      <c r="G51" s="8" t="s">
+        <v>18</v>
       </c>
       <c r="H51">
         <v>0.08</v>
@@ -2674,7 +2674,7 @@
       <c r="I51">
         <v>0</v>
       </c>
-      <c r="J51" s="11">
+      <c r="J51" s="8">
         <v>0</v>
       </c>
       <c r="K51">
@@ -2695,16 +2695,16 @@
         <v>10</v>
       </c>
       <c r="D52" t="s">
-        <v>83</v>
-      </c>
-      <c r="E52" s="11" t="s">
-        <v>84</v>
+        <v>82</v>
+      </c>
+      <c r="E52" s="8" t="s">
+        <v>83</v>
       </c>
       <c r="F52" t="s">
-        <v>12</v>
-      </c>
-      <c r="G52" s="11" t="s">
-        <v>19</v>
+        <v>11</v>
+      </c>
+      <c r="G52" s="8" t="s">
+        <v>18</v>
       </c>
       <c r="H52">
         <v>0.12</v>
@@ -2712,7 +2712,7 @@
       <c r="I52">
         <v>0</v>
       </c>
-      <c r="J52" s="11">
+      <c r="J52" s="8">
         <v>0</v>
       </c>
       <c r="K52">
@@ -2733,16 +2733,16 @@
         <v>2</v>
       </c>
       <c r="D53" t="s">
-        <v>82</v>
-      </c>
-      <c r="E53" s="11" t="s">
-        <v>84</v>
+        <v>81</v>
+      </c>
+      <c r="E53" s="8" t="s">
+        <v>83</v>
       </c>
       <c r="F53" t="s">
-        <v>12</v>
-      </c>
-      <c r="G53" s="11" t="s">
-        <v>12</v>
+        <v>11</v>
+      </c>
+      <c r="G53" s="8" t="s">
+        <v>11</v>
       </c>
       <c r="H53">
         <v>0</v>
@@ -2750,7 +2750,7 @@
       <c r="I53">
         <v>0</v>
       </c>
-      <c r="J53" s="11">
+      <c r="J53" s="8">
         <v>0</v>
       </c>
       <c r="K53">
@@ -2771,16 +2771,16 @@
         <v>4</v>
       </c>
       <c r="D54" t="s">
-        <v>82</v>
-      </c>
-      <c r="E54" s="11" t="s">
-        <v>84</v>
+        <v>81</v>
+      </c>
+      <c r="E54" s="8" t="s">
+        <v>83</v>
       </c>
       <c r="F54" t="s">
-        <v>12</v>
-      </c>
-      <c r="G54" s="11" t="s">
-        <v>12</v>
+        <v>11</v>
+      </c>
+      <c r="G54" s="8" t="s">
+        <v>11</v>
       </c>
       <c r="H54">
         <v>0.02</v>
@@ -2788,7 +2788,7 @@
       <c r="I54">
         <v>0</v>
       </c>
-      <c r="J54" s="11">
+      <c r="J54" s="8">
         <v>0</v>
       </c>
       <c r="K54">
@@ -2809,16 +2809,16 @@
         <v>6</v>
       </c>
       <c r="D55" t="s">
-        <v>82</v>
-      </c>
-      <c r="E55" s="11" t="s">
-        <v>84</v>
+        <v>81</v>
+      </c>
+      <c r="E55" s="8" t="s">
+        <v>83</v>
       </c>
       <c r="F55" t="s">
-        <v>12</v>
-      </c>
-      <c r="G55" s="11" t="s">
-        <v>12</v>
+        <v>11</v>
+      </c>
+      <c r="G55" s="8" t="s">
+        <v>11</v>
       </c>
       <c r="H55">
         <v>0.03</v>
@@ -2826,7 +2826,7 @@
       <c r="I55">
         <v>0</v>
       </c>
-      <c r="J55" s="11">
+      <c r="J55" s="8">
         <v>0</v>
       </c>
       <c r="K55">
@@ -2847,16 +2847,16 @@
         <v>8</v>
       </c>
       <c r="D56" t="s">
-        <v>82</v>
-      </c>
-      <c r="E56" s="11" t="s">
-        <v>84</v>
+        <v>81</v>
+      </c>
+      <c r="E56" s="8" t="s">
+        <v>83</v>
       </c>
       <c r="F56" t="s">
-        <v>12</v>
-      </c>
-      <c r="G56" s="11" t="s">
-        <v>19</v>
+        <v>11</v>
+      </c>
+      <c r="G56" s="8" t="s">
+        <v>18</v>
       </c>
       <c r="H56">
         <v>0.06</v>
@@ -2864,7 +2864,7 @@
       <c r="I56">
         <v>0</v>
       </c>
-      <c r="J56" s="11">
+      <c r="J56" s="8">
         <v>0</v>
       </c>
       <c r="K56">
@@ -2885,16 +2885,16 @@
         <v>10</v>
       </c>
       <c r="D57" t="s">
-        <v>82</v>
-      </c>
-      <c r="E57" s="11" t="s">
-        <v>84</v>
+        <v>81</v>
+      </c>
+      <c r="E57" s="8" t="s">
+        <v>83</v>
       </c>
       <c r="F57" t="s">
-        <v>12</v>
-      </c>
-      <c r="G57" s="11" t="s">
-        <v>12</v>
+        <v>11</v>
+      </c>
+      <c r="G57" s="8" t="s">
+        <v>11</v>
       </c>
       <c r="H57">
         <v>0.1</v>
@@ -2902,7 +2902,7 @@
       <c r="I57">
         <v>0</v>
       </c>
-      <c r="J57" s="11">
+      <c r="J57" s="8">
         <v>0</v>
       </c>
       <c r="K57">
@@ -2923,24 +2923,24 @@
         <v>2</v>
       </c>
       <c r="D58" t="s">
-        <v>81</v>
-      </c>
-      <c r="E58" s="11" t="s">
-        <v>84</v>
+        <v>80</v>
+      </c>
+      <c r="E58" s="8" t="s">
+        <v>83</v>
       </c>
       <c r="F58" t="s">
+        <v>62</v>
+      </c>
+      <c r="G58" s="8" t="s">
         <v>63</v>
       </c>
-      <c r="G58" s="11" t="s">
-        <v>64</v>
-      </c>
       <c r="H58">
         <v>0</v>
       </c>
       <c r="I58">
         <v>0</v>
       </c>
-      <c r="J58" s="11">
+      <c r="J58" s="8">
         <v>0</v>
       </c>
       <c r="K58">
@@ -2961,16 +2961,16 @@
         <v>4</v>
       </c>
       <c r="D59" t="s">
-        <v>81</v>
-      </c>
-      <c r="E59" s="11" t="s">
-        <v>84</v>
+        <v>80</v>
+      </c>
+      <c r="E59" s="8" t="s">
+        <v>83</v>
       </c>
       <c r="F59" t="s">
+        <v>64</v>
+      </c>
+      <c r="G59" s="8" t="s">
         <v>65</v>
-      </c>
-      <c r="G59" s="11" t="s">
-        <v>66</v>
       </c>
       <c r="H59">
         <v>0.01</v>
@@ -2978,7 +2978,7 @@
       <c r="I59">
         <v>0</v>
       </c>
-      <c r="J59" s="11">
+      <c r="J59" s="8">
         <v>0</v>
       </c>
       <c r="K59">
@@ -2999,16 +2999,16 @@
         <v>6</v>
       </c>
       <c r="D60" t="s">
-        <v>81</v>
-      </c>
-      <c r="E60" s="11" t="s">
-        <v>84</v>
+        <v>80</v>
+      </c>
+      <c r="E60" s="8" t="s">
+        <v>83</v>
       </c>
       <c r="F60" t="s">
-        <v>67</v>
-      </c>
-      <c r="G60" s="11" t="s">
-        <v>38</v>
+        <v>66</v>
+      </c>
+      <c r="G60" s="8" t="s">
+        <v>37</v>
       </c>
       <c r="H60">
         <v>0.02</v>
@@ -3016,7 +3016,7 @@
       <c r="I60">
         <v>0</v>
       </c>
-      <c r="J60" s="11">
+      <c r="J60" s="8">
         <v>0</v>
       </c>
       <c r="K60">
@@ -3037,16 +3037,16 @@
         <v>8</v>
       </c>
       <c r="D61" t="s">
-        <v>81</v>
-      </c>
-      <c r="E61" s="11" t="s">
-        <v>84</v>
+        <v>80</v>
+      </c>
+      <c r="E61" s="8" t="s">
+        <v>83</v>
       </c>
       <c r="F61" t="s">
+        <v>67</v>
+      </c>
+      <c r="G61" s="8" t="s">
         <v>68</v>
-      </c>
-      <c r="G61" s="11" t="s">
-        <v>69</v>
       </c>
       <c r="H61">
         <v>0.03</v>
@@ -3054,7 +3054,7 @@
       <c r="I61">
         <v>0</v>
       </c>
-      <c r="J61" s="11">
+      <c r="J61" s="8">
         <v>0</v>
       </c>
       <c r="K61">
@@ -3075,16 +3075,16 @@
         <v>10</v>
       </c>
       <c r="D62" t="s">
-        <v>81</v>
-      </c>
-      <c r="E62" s="11" t="s">
-        <v>84</v>
+        <v>80</v>
+      </c>
+      <c r="E62" s="8" t="s">
+        <v>83</v>
       </c>
       <c r="F62" t="s">
-        <v>70</v>
-      </c>
-      <c r="G62" s="11" t="s">
-        <v>68</v>
+        <v>69</v>
+      </c>
+      <c r="G62" s="8" t="s">
+        <v>67</v>
       </c>
       <c r="H62">
         <v>0.06</v>
@@ -3092,7 +3092,7 @@
       <c r="I62">
         <v>0</v>
       </c>
-      <c r="J62" s="11">
+      <c r="J62" s="8">
         <v>0</v>
       </c>
       <c r="K62">
@@ -3113,16 +3113,16 @@
         <v>2</v>
       </c>
       <c r="D63" t="s">
-        <v>83</v>
-      </c>
-      <c r="E63" s="11" t="s">
-        <v>84</v>
+        <v>82</v>
+      </c>
+      <c r="E63" s="8" t="s">
+        <v>83</v>
       </c>
       <c r="F63" t="s">
-        <v>12</v>
-      </c>
-      <c r="G63" s="11" t="s">
-        <v>71</v>
+        <v>11</v>
+      </c>
+      <c r="G63" s="8" t="s">
+        <v>70</v>
       </c>
       <c r="H63">
         <v>0</v>
@@ -3130,7 +3130,7 @@
       <c r="I63">
         <v>0</v>
       </c>
-      <c r="J63" s="11">
+      <c r="J63" s="8">
         <v>0</v>
       </c>
       <c r="K63">
@@ -3151,16 +3151,16 @@
         <v>4</v>
       </c>
       <c r="D64" t="s">
-        <v>83</v>
-      </c>
-      <c r="E64" s="11" t="s">
-        <v>84</v>
+        <v>82</v>
+      </c>
+      <c r="E64" s="8" t="s">
+        <v>83</v>
       </c>
       <c r="F64" t="s">
-        <v>12</v>
-      </c>
-      <c r="G64" s="11" t="s">
-        <v>72</v>
+        <v>11</v>
+      </c>
+      <c r="G64" s="8" t="s">
+        <v>71</v>
       </c>
       <c r="H64">
         <v>0</v>
@@ -3168,7 +3168,7 @@
       <c r="I64">
         <v>0</v>
       </c>
-      <c r="J64" s="11">
+      <c r="J64" s="8">
         <v>0</v>
       </c>
       <c r="K64">
@@ -3189,16 +3189,16 @@
         <v>6</v>
       </c>
       <c r="D65" t="s">
-        <v>83</v>
-      </c>
-      <c r="E65" s="11" t="s">
-        <v>84</v>
+        <v>82</v>
+      </c>
+      <c r="E65" s="8" t="s">
+        <v>83</v>
       </c>
       <c r="F65" t="s">
-        <v>12</v>
-      </c>
-      <c r="G65" s="11" t="s">
-        <v>36</v>
+        <v>11</v>
+      </c>
+      <c r="G65" s="8" t="s">
+        <v>35</v>
       </c>
       <c r="H65">
         <v>0</v>
@@ -3206,7 +3206,7 @@
       <c r="I65">
         <v>0</v>
       </c>
-      <c r="J65" s="11">
+      <c r="J65" s="8">
         <v>0</v>
       </c>
       <c r="K65">
@@ -3227,16 +3227,16 @@
         <v>8</v>
       </c>
       <c r="D66" t="s">
-        <v>83</v>
-      </c>
-      <c r="E66" s="11" t="s">
-        <v>84</v>
+        <v>82</v>
+      </c>
+      <c r="E66" s="8" t="s">
+        <v>83</v>
       </c>
       <c r="F66" t="s">
-        <v>12</v>
-      </c>
-      <c r="G66" s="11" t="s">
-        <v>73</v>
+        <v>11</v>
+      </c>
+      <c r="G66" s="8" t="s">
+        <v>72</v>
       </c>
       <c r="H66">
         <v>0.01</v>
@@ -3244,7 +3244,7 @@
       <c r="I66">
         <v>0</v>
       </c>
-      <c r="J66" s="11">
+      <c r="J66" s="8">
         <v>0</v>
       </c>
       <c r="K66">
@@ -3265,16 +3265,16 @@
         <v>10</v>
       </c>
       <c r="D67" t="s">
-        <v>83</v>
-      </c>
-      <c r="E67" s="11" t="s">
-        <v>84</v>
+        <v>82</v>
+      </c>
+      <c r="E67" s="8" t="s">
+        <v>83</v>
       </c>
       <c r="F67" t="s">
-        <v>12</v>
-      </c>
-      <c r="G67" s="11" t="s">
-        <v>74</v>
+        <v>11</v>
+      </c>
+      <c r="G67" s="8" t="s">
+        <v>73</v>
       </c>
       <c r="H67">
         <v>0.01</v>
@@ -3282,7 +3282,7 @@
       <c r="I67">
         <v>0</v>
       </c>
-      <c r="J67" s="11">
+      <c r="J67" s="8">
         <v>0</v>
       </c>
       <c r="K67">
@@ -3303,16 +3303,16 @@
         <v>2</v>
       </c>
       <c r="D68" t="s">
-        <v>82</v>
-      </c>
-      <c r="E68" s="11" t="s">
-        <v>84</v>
+        <v>81</v>
+      </c>
+      <c r="E68" s="8" t="s">
+        <v>83</v>
       </c>
       <c r="F68" t="s">
-        <v>12</v>
-      </c>
-      <c r="G68" s="11" t="s">
-        <v>12</v>
+        <v>11</v>
+      </c>
+      <c r="G68" s="8" t="s">
+        <v>11</v>
       </c>
       <c r="H68">
         <v>0</v>
@@ -3320,7 +3320,7 @@
       <c r="I68">
         <v>0</v>
       </c>
-      <c r="J68" s="11">
+      <c r="J68" s="8">
         <v>0</v>
       </c>
       <c r="K68">
@@ -3341,16 +3341,16 @@
         <v>4</v>
       </c>
       <c r="D69" t="s">
-        <v>82</v>
-      </c>
-      <c r="E69" s="11" t="s">
-        <v>84</v>
+        <v>81</v>
+      </c>
+      <c r="E69" s="8" t="s">
+        <v>83</v>
       </c>
       <c r="F69" t="s">
-        <v>12</v>
-      </c>
-      <c r="G69" s="11" t="s">
-        <v>12</v>
+        <v>11</v>
+      </c>
+      <c r="G69" s="8" t="s">
+        <v>11</v>
       </c>
       <c r="H69">
         <v>0</v>
@@ -3358,7 +3358,7 @@
       <c r="I69">
         <v>0</v>
       </c>
-      <c r="J69" s="11">
+      <c r="J69" s="8">
         <v>0</v>
       </c>
       <c r="K69">
@@ -3379,16 +3379,16 @@
         <v>6</v>
       </c>
       <c r="D70" t="s">
-        <v>82</v>
-      </c>
-      <c r="E70" s="11" t="s">
-        <v>84</v>
+        <v>81</v>
+      </c>
+      <c r="E70" s="8" t="s">
+        <v>83</v>
       </c>
       <c r="F70" t="s">
-        <v>12</v>
-      </c>
-      <c r="G70" s="11" t="s">
-        <v>12</v>
+        <v>11</v>
+      </c>
+      <c r="G70" s="8" t="s">
+        <v>11</v>
       </c>
       <c r="H70">
         <v>0</v>
@@ -3396,7 +3396,7 @@
       <c r="I70">
         <v>0</v>
       </c>
-      <c r="J70" s="11">
+      <c r="J70" s="8">
         <v>0</v>
       </c>
       <c r="K70">
@@ -3417,16 +3417,16 @@
         <v>8</v>
       </c>
       <c r="D71" t="s">
-        <v>82</v>
-      </c>
-      <c r="E71" s="11" t="s">
-        <v>84</v>
+        <v>81</v>
+      </c>
+      <c r="E71" s="8" t="s">
+        <v>83</v>
       </c>
       <c r="F71" t="s">
-        <v>12</v>
-      </c>
-      <c r="G71" s="11" t="s">
-        <v>12</v>
+        <v>11</v>
+      </c>
+      <c r="G71" s="8" t="s">
+        <v>11</v>
       </c>
       <c r="H71">
         <v>0.01</v>
@@ -3434,7 +3434,7 @@
       <c r="I71">
         <v>0</v>
       </c>
-      <c r="J71" s="11">
+      <c r="J71" s="8">
         <v>0</v>
       </c>
       <c r="K71">
@@ -3455,16 +3455,16 @@
         <v>10</v>
       </c>
       <c r="D72" t="s">
-        <v>82</v>
-      </c>
-      <c r="E72" s="11" t="s">
-        <v>84</v>
+        <v>81</v>
+      </c>
+      <c r="E72" s="8" t="s">
+        <v>83</v>
       </c>
       <c r="F72" t="s">
-        <v>12</v>
-      </c>
-      <c r="G72" s="11" t="s">
-        <v>12</v>
+        <v>11</v>
+      </c>
+      <c r="G72" s="8" t="s">
+        <v>11</v>
       </c>
       <c r="H72">
         <v>0.01</v>
@@ -3472,7 +3472,7 @@
       <c r="I72">
         <v>0</v>
       </c>
-      <c r="J72" s="11">
+      <c r="J72" s="8">
         <v>0</v>
       </c>
       <c r="K72">
@@ -3493,24 +3493,24 @@
         <v>2</v>
       </c>
       <c r="D73" t="s">
-        <v>81</v>
-      </c>
-      <c r="E73" s="11" t="s">
-        <v>84</v>
+        <v>80</v>
+      </c>
+      <c r="E73" s="8" t="s">
+        <v>83</v>
       </c>
       <c r="F73" t="s">
-        <v>73</v>
-      </c>
-      <c r="G73" s="11" t="s">
         <v>72</v>
       </c>
+      <c r="G73" s="8" t="s">
+        <v>71</v>
+      </c>
       <c r="H73">
         <v>0</v>
       </c>
       <c r="I73">
         <v>0</v>
       </c>
-      <c r="J73" s="11">
+      <c r="J73" s="8">
         <v>0</v>
       </c>
       <c r="K73">
@@ -3531,16 +3531,16 @@
         <v>4</v>
       </c>
       <c r="D74" t="s">
-        <v>81</v>
-      </c>
-      <c r="E74" s="11" t="s">
-        <v>84</v>
+        <v>80</v>
+      </c>
+      <c r="E74" s="8" t="s">
+        <v>83</v>
       </c>
       <c r="F74" t="s">
-        <v>73</v>
-      </c>
-      <c r="G74" s="11" t="s">
-        <v>75</v>
+        <v>72</v>
+      </c>
+      <c r="G74" s="8" t="s">
+        <v>74</v>
       </c>
       <c r="H74">
         <v>0</v>
@@ -3548,7 +3548,7 @@
       <c r="I74">
         <v>0</v>
       </c>
-      <c r="J74" s="11">
+      <c r="J74" s="8">
         <v>0</v>
       </c>
       <c r="K74">
@@ -3569,24 +3569,24 @@
         <v>6</v>
       </c>
       <c r="D75" t="s">
-        <v>81</v>
-      </c>
-      <c r="E75" s="11" t="s">
-        <v>84</v>
+        <v>80</v>
+      </c>
+      <c r="E75" s="8" t="s">
+        <v>83</v>
       </c>
       <c r="F75" t="s">
+        <v>75</v>
+      </c>
+      <c r="G75" s="8" t="s">
         <v>76</v>
       </c>
-      <c r="G75" s="11" t="s">
-        <v>77</v>
-      </c>
       <c r="H75">
         <v>0</v>
       </c>
       <c r="I75">
         <v>0</v>
       </c>
-      <c r="J75" s="11">
+      <c r="J75" s="8">
         <v>0</v>
       </c>
       <c r="K75">
@@ -3607,16 +3607,16 @@
         <v>8</v>
       </c>
       <c r="D76" t="s">
-        <v>81</v>
-      </c>
-      <c r="E76" s="11" t="s">
-        <v>84</v>
+        <v>80</v>
+      </c>
+      <c r="E76" s="8" t="s">
+        <v>83</v>
       </c>
       <c r="F76" t="s">
-        <v>78</v>
-      </c>
-      <c r="G76" s="11" t="s">
-        <v>36</v>
+        <v>77</v>
+      </c>
+      <c r="G76" s="8" t="s">
+        <v>35</v>
       </c>
       <c r="H76">
         <v>0.01</v>
@@ -3624,7 +3624,7 @@
       <c r="I76">
         <v>0</v>
       </c>
-      <c r="J76" s="11">
+      <c r="J76" s="8">
         <v>0</v>
       </c>
       <c r="K76">
@@ -3635,40 +3635,40 @@
       </c>
     </row>
     <row r="77" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A77" s="8">
-        <v>100</v>
-      </c>
-      <c r="B77" s="8">
+      <c r="A77" s="5">
+        <v>100</v>
+      </c>
+      <c r="B77" s="5">
         <v>1000</v>
       </c>
-      <c r="C77" s="8">
+      <c r="C77" s="5">
         <v>10</v>
       </c>
-      <c r="D77" s="8" t="s">
-        <v>81</v>
-      </c>
-      <c r="E77" s="12" t="s">
-        <v>84</v>
-      </c>
-      <c r="F77" s="8" t="s">
+      <c r="D77" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="E77" s="9" t="s">
+        <v>83</v>
+      </c>
+      <c r="F77" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="G77" s="9" t="s">
         <v>79</v>
       </c>
-      <c r="G77" s="12" t="s">
-        <v>80</v>
-      </c>
-      <c r="H77" s="8">
+      <c r="H77" s="5">
         <v>0.01</v>
       </c>
-      <c r="I77" s="8">
-        <v>0</v>
-      </c>
-      <c r="J77" s="12">
-        <v>0</v>
-      </c>
-      <c r="K77" s="8">
+      <c r="I77" s="5">
+        <v>0</v>
+      </c>
+      <c r="J77" s="9">
+        <v>0</v>
+      </c>
+      <c r="K77" s="5">
         <v>3.28</v>
       </c>
-      <c r="L77" s="8">
+      <c r="L77" s="5">
         <v>4.07</v>
       </c>
     </row>

</xml_diff>